<commit_message>
automize the making of the parameter tables.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/calibration.xlsx
+++ b/WorkingFolder/Tables/calibration.xlsx
@@ -14,57 +14,162 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+  <si>
+    <t>parameter name</t>
+  </si>
   <si>
     <t>values</t>
   </si>
   <si>
-    <t>('risk', 'σ_ψ')</t>
-  </si>
-  <si>
-    <t>('risk', 'σ_θ')</t>
-  </si>
-  <si>
-    <t>('risk', 'U2U')</t>
-  </si>
-  <si>
-    <t>('risk', 'E2E')</t>
-  </si>
-  <si>
-    <t>('initial condition', 'σ_ψ_init')</t>
-  </si>
-  <si>
-    <t>('initial condition', 'init_b')</t>
-  </si>
-  <si>
-    <t>('initial condition', 'bequest_ratio')</t>
-  </si>
-  <si>
-    <t>('life-cycle', 'T')</t>
-  </si>
-  <si>
-    <t>('life-cycle', 'L')</t>
-  </si>
-  <si>
-    <t>('life-cycle', '1-D')</t>
-  </si>
-  <si>
-    <t>('preference', 'ρ')</t>
-  </si>
-  <si>
-    <t>('preference', 'β')</t>
-  </si>
-  <si>
-    <t>('policy', 'λ')</t>
-  </si>
-  <si>
-    <t>('policy', 'λ_SS')</t>
-  </si>
-  <si>
-    <t>('policy', 'transfer')</t>
-  </si>
-  <si>
-    <t>('policy', 'μ')</t>
+    <t>source</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>risk</t>
+  </si>
+  <si>
+    <t>initial condition</t>
+  </si>
+  <si>
+    <t>life cycle</t>
+  </si>
+  <si>
+    <t>preference</t>
+  </si>
+  <si>
+    <t>policy</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>σ_ψ</t>
+  </si>
+  <si>
+    <t>σ_θ</t>
+  </si>
+  <si>
+    <t>U2U</t>
+  </si>
+  <si>
+    <t>E2E</t>
+  </si>
+  <si>
+    <t>σ_ψ_init</t>
+  </si>
+  <si>
+    <t>bequest_ratio</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>1-D</t>
+  </si>
+  <si>
+    <t>ρ</t>
+  </si>
+  <si>
+    <t>β</t>
+  </si>
+  <si>
+    <t>λ</t>
+  </si>
+  <si>
+    <t>λ_SS</t>
+  </si>
+  <si>
+    <t>μ</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>K2Y ratio</t>
+  </si>
+  <si>
+    <t>α</t>
+  </si>
+  <si>
+    <t>δ</t>
+  </si>
+  <si>
+    <t>$\sigma_\psi$</t>
+  </si>
+  <si>
+    <t>$\sigma_	heta$</t>
+  </si>
+  <si>
+    <t>$U2U$</t>
+  </si>
+  <si>
+    <t>$E2E$</t>
+  </si>
+  <si>
+    <t>$\sigma_\psi^{\text{init}}$</t>
+  </si>
+  <si>
+    <t>bequest ratio</t>
+  </si>
+  <si>
+    <t>$T$</t>
+  </si>
+  <si>
+    <t>$L$</t>
+  </si>
+  <si>
+    <t>$1-D$</t>
+  </si>
+  <si>
+    <t>$\rho$</t>
+  </si>
+  <si>
+    <t>$\beta$</t>
+  </si>
+  <si>
+    <t>$\lambda$</t>
+  </si>
+  <si>
+    <t>$\lambda_{SS}$</t>
+  </si>
+  <si>
+    <t>$\mu$</t>
+  </si>
+  <si>
+    <t>$W$</t>
+  </si>
+  <si>
+    <t>$\alpha$</t>
+  </si>
+  <si>
+    <t>$\delta$</t>
+  </si>
+  <si>
+    <t>Median estimates from the literature</t>
+  </si>
+  <si>
+    <t>Estimated for age 25 in the 2016 SCF</t>
+  </si>
+  <si>
+    <t>assumption</t>
+  </si>
+  <si>
+    <t>standard assumption</t>
+  </si>
+  <si>
+    <t>endogenously determined</t>
+  </si>
+  <si>
+    <t>target values in steady state</t>
   </si>
 </sst>
 </file>
@@ -422,146 +527,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6">
         <v>0.629</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>0.554</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10">
+        <v>0.994</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>1.5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12">
+        <v>0.98</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15">
+        <v>0.15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>0.994</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>0.15</v>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18">
+        <v>0.33</v>
+      </c>
+      <c r="E18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19">
+        <v>0.025</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
temporarily finalize on calibration of objective model results. seaborn style plot. need to debug retirement kink still.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/calibration.xlsx
+++ b/WorkingFolder/Tables/calibration.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>parameter name</t>
   </si>
@@ -79,6 +79,9 @@
     <t>$\beta$</t>
   </si>
   <si>
+    <t>$\mathbb{S}$</t>
+  </si>
+  <si>
     <t>$\lambda$</t>
   </si>
   <si>
@@ -110,6 +113,9 @@
   </si>
   <si>
     <t>standard assumption</t>
+  </si>
+  <si>
+    <t>U.S. average</t>
   </si>
   <si>
     <t>endogenously determined</t>
@@ -473,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -504,7 +510,7 @@
         <v>0.15</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -518,7 +524,7 @@
         <v>0.1</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -532,7 +538,7 @@
         <v>0.18</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -546,7 +552,7 @@
         <v>0.96</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -560,7 +566,7 @@
         <v>0.629</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -574,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -588,7 +594,7 @@
         <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -602,7 +608,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -616,7 +622,7 @@
         <v>0.994</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -627,10 +633,10 @@
         <v>19</v>
       </c>
       <c r="C11">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -644,7 +650,7 @@
         <v>0.98</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -655,10 +661,10 @@
         <v>21</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -672,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -683,21 +689,21 @@
         <v>23</v>
       </c>
       <c r="C15">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>24</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="D16" t="s">
         <v>33</v>
@@ -711,10 +717,10 @@
         <v>25</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -725,10 +731,10 @@
         <v>26</v>
       </c>
       <c r="C18">
-        <v>0.33</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -739,10 +745,24 @@
         <v>27</v>
       </c>
       <c r="C19">
+        <v>0.33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20">
         <v>0.025</v>
       </c>
-      <c r="D19" t="s">
-        <v>31</v>
+      <c r="D20" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rename AggregateDynamics to OLG-GE. add two more attributes differentiating subjective sigmas and objective sigmas. Now simulation is always based on true sigmas.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/calibration.xlsx
+++ b/WorkingFolder/Tables/calibration.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>parameter name</t>
   </si>
@@ -46,6 +46,9 @@
     <t>production</t>
   </si>
   <si>
+    <t>subjective</t>
+  </si>
+  <si>
     <t>$\sigma_\psi$</t>
   </si>
   <si>
@@ -103,6 +106,12 @@
     <t>$\delta$</t>
   </si>
   <si>
+    <t>$\sigma_\psi^{\text{sub}}$</t>
+  </si>
+  <si>
+    <t>$\sigma_\theta^{\text{sub}}$</t>
+  </si>
+  <si>
     <t>Median estimates from the literature</t>
   </si>
   <si>
@@ -122,6 +131,9 @@
   </si>
   <si>
     <t>target values in steady state</t>
+  </si>
+  <si>
+    <t>estimated from SCE</t>
   </si>
 </sst>
 </file>
@@ -479,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -504,13 +516,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>0.15</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -518,13 +530,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>0.1</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -532,13 +544,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>0.18</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -546,13 +558,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>0.96</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -560,13 +572,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>0.629</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -574,13 +586,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -588,13 +600,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -602,13 +614,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -616,13 +628,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>0.994</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -630,13 +642,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -644,13 +656,13 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>0.98</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -658,13 +670,13 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>0.65</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -672,13 +684,13 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -686,13 +698,13 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -700,13 +712,13 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16">
         <v>0.15</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -714,13 +726,13 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -728,13 +740,13 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -742,13 +754,13 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19">
         <v>0.33</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -756,13 +768,41 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20">
         <v>0.025</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21">
+        <v>0.03457920401687286</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>0.02010668171428303</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated graphs and tables from Stata
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/calibration.xlsx
+++ b/WorkingFolder/Tables/calibration.xlsx
@@ -779,7 +779,7 @@
         <v>30</v>
       </c>
       <c r="C21">
-        <v>0.03533719439759439</v>
+        <v>0.03478873974423526</v>
       </c>
       <c r="D21" t="s">
         <v>39</v>
@@ -793,7 +793,7 @@
         <v>31</v>
       </c>
       <c r="C22">
-        <v>0.01874253697092856</v>
+        <v>0.01974192460242583</v>
       </c>
       <c r="D22" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Solve life cycle now can handle age-specific survival probs. OLG-GE needs to be revised to accomodate this change.
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/calibration.xlsx
+++ b/WorkingFolder/Tables/calibration.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>parameter name</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>$L$</t>
-  </si>
-  <si>
-    <t>$1-D$</t>
   </si>
   <si>
     <t>$\rho$</t>
@@ -494,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -525,7 +522,7 @@
         <v>0.15</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -539,7 +536,7 @@
         <v>0.15</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -553,7 +550,7 @@
         <v>0.18</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -567,7 +564,7 @@
         <v>0.96</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -581,7 +578,7 @@
         <v>0.629</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -595,7 +592,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -609,7 +606,7 @@
         <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -623,21 +620,21 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
       <c r="C10">
-        <v>0.994</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -648,7 +645,7 @@
         <v>20</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>0.97</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -656,13 +653,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="C12">
-        <v>0.97</v>
+        <v>0.65</v>
       </c>
       <c r="D12" t="s">
         <v>36</v>
@@ -675,9 +672,6 @@
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C13">
-        <v>0.65</v>
-      </c>
       <c r="D13" t="s">
         <v>37</v>
       </c>
@@ -690,7 +684,7 @@
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -700,22 +694,25 @@
       <c r="B15" t="s">
         <v>24</v>
       </c>
+      <c r="C15">
+        <v>0.15</v>
+      </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
       <c r="C16">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -726,10 +723,10 @@
         <v>26</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -740,10 +737,10 @@
         <v>27</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>0.33</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -754,24 +751,24 @@
         <v>28</v>
       </c>
       <c r="C19">
-        <v>0.33</v>
+        <v>0.025</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
         <v>29</v>
       </c>
       <c r="C20">
-        <v>0.025</v>
+        <v>0.03532417840887617</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -782,24 +779,10 @@
         <v>30</v>
       </c>
       <c r="C21">
-        <v>0.03478874032651719</v>
+        <v>0.01876705676812129</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22">
-        <v>0.01974192357634271</v>
-      </c>
-      <c r="D22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added population growth positive in calibration in table
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/calibration.xlsx
+++ b/WorkingFolder/Tables/calibration.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,15 +583,15 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>$T$</t>
+          <t>$n$</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>40</v>
+        <v>0.005</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>standard calibration</t>
+          <t>U.S. Census</t>
         </is>
       </c>
     </row>
@@ -603,11 +603,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>$L$</t>
+          <t>$T$</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -618,16 +618,16 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>preference</t>
+          <t>life cycle</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>$\rho$</t>
+          <t>$L$</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -643,35 +643,35 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>$\beta$</t>
+          <t>$\rho$</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.97</v>
+        <v>2</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>calibrated to match average wealth/income ratio</t>
+          <t>standard calibration</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>policy</t>
+          <t>preference</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>$\mathbb{S}$</t>
+          <t>$\beta$</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.65</v>
+        <v>0.97</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>U.S. average</t>
+          <t>calibrated to match average wealth/income ratio</t>
         </is>
       </c>
     </row>
@@ -683,13 +683,15 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>$\lambda$</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
+          <t>$\mathbb{S}$</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.65</v>
+      </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>endogenously determined</t>
+          <t>U.S. average</t>
         </is>
       </c>
     </row>
@@ -701,13 +703,13 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>$\lambda_{SS}$</t>
+          <t>$\lambda$</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>U.S. average</t>
+          <t>endogenously determined</t>
         </is>
       </c>
     </row>
@@ -719,12 +721,10 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>$\mu$</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0.15</v>
-      </c>
+          <t>$\lambda_{SS}$</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
           <t>U.S. average</t>
@@ -734,20 +734,20 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>production</t>
+          <t>policy</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>$W$</t>
+          <t>$\mu$</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>target values in steady state</t>
+          <t>U.S. average</t>
         </is>
       </c>
     </row>
@@ -759,11 +759,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>K2Y ratio</t>
+          <t>$W$</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -779,15 +779,15 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>$\alpha$</t>
+          <t>K2Y ratio</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.33</v>
+        <v>3</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>standard calibration</t>
+          <t>target values in steady state</t>
         </is>
       </c>
     </row>
@@ -799,11 +799,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>$\delta$</t>
+          <t>$\alpha$</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.025</v>
+        <v>0.33</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -814,20 +814,20 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>subjective</t>
+          <t>production</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>$\sigma_\psi^{\text{sub}}$</t>
+          <t>$\delta$</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.0343116236669084</v>
+        <v>0.025</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>estimated from SCE</t>
+          <t>standard calibration</t>
         </is>
       </c>
     </row>
@@ -839,13 +839,33 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>$\sigma_\psi^{\text{sub}}$</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0343116236669084</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>estimated from SCE</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>subjective</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>$\sigma_\theta^{\text{sub}}$</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="C22" t="n">
         <v>0.02055997279522646</v>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>estimated from SCE</t>
         </is>

</xml_diff>

<commit_message>
model summary and calibration for the revised draft
</commit_message>
<xml_diff>
--- a/WorkingFolder/Tables/calibration.xlsx
+++ b/WorkingFolder/Tables/calibration.xlsx
@@ -671,7 +671,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>calibrated to match average wealth/income ratio</t>
+          <t>targeting average wealth/income ratio</t>
         </is>
       </c>
     </row>
@@ -843,7 +843,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.0343116236669084</v>
+        <v>0.03431162453071653</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -863,7 +863,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.02055997279522646</v>
+        <v>0.02055997135365542</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>

</xml_diff>